<commit_message>
search_db_excel found.text bug fixed2
</commit_message>
<xml_diff>
--- a/database/power-int.xlsx
+++ b/database/power-int.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="109">
   <si>
     <t>시간</t>
   </si>
@@ -22,7 +22,325 @@
     <t>적산전력량(kWh)</t>
   </si>
   <si>
-    <t>2015-11-18 18:10</t>
+    <t>2016-03-20 21:10:03.606</t>
+  </si>
+  <si>
+    <t>2016-03-20 21:00:04.729</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:50:02.808</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:40:02.780</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:30:02.434</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:20:04.747</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:10:01.019</t>
+  </si>
+  <si>
+    <t>2016-03-20 20:00:01.491</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:50:01.479</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:40:03.750</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:30:01.771</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:20:04.484</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:10:03.463</t>
+  </si>
+  <si>
+    <t>2016-03-20 19:00:02.433</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:50:04.441</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:40:06.230</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:30:01.457</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:20:03.767</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:10:01.730</t>
+  </si>
+  <si>
+    <t>2016-03-20 18:00:04.448</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:50:03.438</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:40:02.428</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:30:01.476</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:20:03.787</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:10:01.772</t>
+  </si>
+  <si>
+    <t>2016-03-20 17:00:04.426</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:50:03.475</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:40:01.495</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:30:04.111</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:20:01.765</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:10:03.441</t>
+  </si>
+  <si>
+    <t>2016-03-20 16:00:01.713</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:50:03.753</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:40:01.773</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:30:04.432</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:20:02.532</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:10:01.471</t>
+  </si>
+  <si>
+    <t>2016-03-20 15:00:03.730</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:50:01.750</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:40:04.460</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:30:03.450</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:20:01.480</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:10:03.745</t>
+  </si>
+  <si>
+    <t>2016-03-20 14:00:01.858</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:50:03.478</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:40:02.445</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:30:01.439</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:20:03.804</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:10:01.789</t>
+  </si>
+  <si>
+    <t>2016-03-20 13:00:04.444</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:50:03.465</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:40:02.456</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:30:01.475</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:20:03.744</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:10:01.764</t>
+  </si>
+  <si>
+    <t>2016-03-20 12:00:04.452</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:50:03.516</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:40:02.439</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:30:01.436</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:20:03.782</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:10:01.792</t>
+  </si>
+  <si>
+    <t>2016-03-20 11:00:04.433</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:50:03.460</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:40:02.430</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:30:04.756</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:20:02.779</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:10:04.443</t>
+  </si>
+  <si>
+    <t>2016-03-20 10:00:02.498</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:50:04.788</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:40:02.767</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:30:03.889</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:20:02.417</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:10:01.507</t>
+  </si>
+  <si>
+    <t>2016-03-20 09:00:03.746</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:50:01.745</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:40:03.481</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:30:01.544</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:20:03.760</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:10:01.774</t>
+  </si>
+  <si>
+    <t>2016-03-20 08:00:04.434</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:50:03.492</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:40:01.513</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:30:03.722</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:20:01.841</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:10:03.801</t>
+  </si>
+  <si>
+    <t>2016-03-20 07:00:02.329</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:50:04.811</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:40:02.910</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:30:04.470</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:20:03.489</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:10:02.469</t>
+  </si>
+  <si>
+    <t>2016-03-20 06:00:01.428</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:50:03.788</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:40:01.767</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:30:04.487</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:20:03.484</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:10:02.466</t>
+  </si>
+  <si>
+    <t>2016-03-20 05:00:01.456</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:50:03.725</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:40:01.765</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:30:04.514</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:20:03.454</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:10:02.434</t>
+  </si>
+  <si>
+    <t>2016-03-20 04:00:01.439</t>
+  </si>
+  <si>
+    <t>2016-03-20 03:50:03.801</t>
+  </si>
+  <si>
+    <t>2016-03-20 03:40:04.881</t>
+  </si>
+  <si>
+    <t>2016-03-20 03:30:04.292</t>
   </si>
 </sst>
 </file>
@@ -368,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,7 +709,855 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>3.87</v>
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="2">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="2">
+        <v>99.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>